<commit_message>
Manually added fenestration subsurfaces to envelope test JSON while I work out how to address dict/lists buried within lists.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_tests_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_tests_draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C541159-E31D-4210-BA6A-EB626F529857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429C0C5E-F912-4DF3-BDA6-C92D381361C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="102">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -315,6 +315,41 @@
   </si>
   <si>
     <t>rule-5-7e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For building area types included in Table G3.1.1-1, vertical fenestration areas for new buildings and additions shall equal that in Table G3.1.1-1 based on the area of gross above-grade walls that separate conditioned spaces and semiheated spaces from the exterior. Where a building has multiple building area types, each type shall use the values in the table. </t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>MISSING_MULTIFAMILY_ENUM</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- For building areas not shown in Table G3.1.1-1, vertical fenestration areas for new buildings and additions shall equal that in the proposed design or 40% of gross above-grade wall area, whichever is smaller, 
+- The vertical fenestration shall be distributed on each face of the building in the same proportion as in the proposed design. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For building areas not shown in Table G3.1.1-1, vertical fenestration areas for new buildings and additions shall equal that in the proposed design or 40% of gross above-grade wall area, whichever is smaller, 
+- The vertical fenestration shall be distributed on each face of the building in the same proportion as in the proposed design. </t>
+  </si>
+  <si>
+    <t>manual_check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- The fenestration area for an existing building shall equal the existing fenestration area prior to the proposed work </t>
+  </si>
+  <si>
+    <t>vertical fenestration area in the proposed design must be as-designed</t>
   </si>
 </sst>
 </file>
@@ -352,7 +387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -501,10 +542,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,8 +898,10 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="K32" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,10 +910,7 @@
     <col min="2" max="2" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="43" style="3" customWidth="1"/>
     <col min="10" max="10" width="53.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="47.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="51.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -898,10 +951,22 @@
         <f t="shared" si="0"/>
         <v>rule-5-7e</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="J1" s="5" t="str">
+        <f t="shared" ref="J1:K1" si="1">"rule-"&amp;J2&amp;"-"&amp;J3&amp;J4</f>
+        <v>rule-5-7f</v>
+      </c>
+      <c r="K1" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>rule-5-7g</v>
+      </c>
+      <c r="L1" s="5" t="str">
+        <f t="shared" ref="L1:M1" si="2">"rule-"&amp;L2&amp;"-"&amp;L3&amp;L4</f>
+        <v>rule-5-7h</v>
+      </c>
+      <c r="M1" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>rule-5-7i</v>
+      </c>
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -926,6 +991,18 @@
       <c r="I2" s="3">
         <v>5</v>
       </c>
+      <c r="J2" s="3">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>5</v>
+      </c>
+      <c r="L2" s="3">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -949,6 +1026,18 @@
       <c r="I3" s="3">
         <v>7</v>
       </c>
+      <c r="J3" s="3">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3">
+        <v>7</v>
+      </c>
+      <c r="L3" s="3">
+        <v>7</v>
+      </c>
+      <c r="M3" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
@@ -972,7 +1061,18 @@
       <c r="I4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="J4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -984,14 +1084,30 @@
       <c r="E5" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1004,6 +1120,30 @@
       <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -1012,10 +1152,6 @@
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -1026,10 +1162,9 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="M8" s="22">
+        <v>100300</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -1048,10 +1183,34 @@
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="F9" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="G9" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="I9" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="J9" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="K9" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="L9" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1069,10 +1228,24 @@
       <c r="E10" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="F10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -1090,12 +1263,24 @@
       <c r="E11" s="6">
         <v>1</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
@@ -1116,12 +1301,24 @@
       <c r="E12" s="3">
         <v>9000</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="F12" s="3">
+        <v>9000</v>
+      </c>
+      <c r="G12" s="3">
+        <v>9000</v>
+      </c>
+      <c r="H12" s="3">
+        <v>9000</v>
+      </c>
+      <c r="I12" s="3">
+        <v>9000</v>
+      </c>
+      <c r="J12" s="3">
+        <v>9000</v>
+      </c>
+      <c r="K12" s="3">
+        <v>9000</v>
+      </c>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1138,13 +1335,26 @@
         <v>70</v>
       </c>
       <c r="E13" s="6">
+        <v>320000</v>
+      </c>
+      <c r="F13" s="6">
+        <v>320000</v>
+      </c>
+      <c r="G13" s="6">
+        <v>320000</v>
+      </c>
+      <c r="H13" s="6">
         <v>300000</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="K13" s="6"/>
+      <c r="I13" s="6">
+        <v>300000</v>
+      </c>
+      <c r="J13" s="6">
+        <v>300000</v>
+      </c>
+      <c r="K13" s="6">
+        <v>300000</v>
+      </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
@@ -1165,10 +1375,28 @@
       <c r="E14" s="6">
         <v>1</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6">
+        <v>1</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
@@ -1186,10 +1414,27 @@
       <c r="E15" s="3">
         <v>1000</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="F15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1000</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -1207,10 +1452,27 @@
       <c r="E16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="F16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
@@ -1228,10 +1490,27 @@
       <c r="E17" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="F17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -1249,10 +1528,27 @@
       <c r="E18" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="F18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
@@ -1270,10 +1566,27 @@
       <c r="E19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="F19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
@@ -1291,10 +1604,27 @@
       <c r="E20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="F20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
@@ -1306,13 +1636,15 @@
       <c r="C21" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="M21" s="23"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
@@ -1324,15 +1656,9 @@
       <c r="C22" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>57</v>
       </c>
@@ -1346,10 +1672,10 @@
         <v>68</v>
       </c>
       <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
       <c r="L23" s="19"/>
@@ -1369,10 +1695,6 @@
       <c r="D24" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
@@ -1388,10 +1710,10 @@
         <v>66</v>
       </c>
       <c r="E25" s="6"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
@@ -1406,10 +1728,6 @@
       <c r="D26" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
@@ -1425,10 +1743,10 @@
         <v>70</v>
       </c>
       <c r="E27" s="6"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
@@ -1444,10 +1762,10 @@
         <v>66</v>
       </c>
       <c r="E28" s="6"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
@@ -1462,10 +1780,6 @@
       <c r="D29" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
@@ -1480,10 +1794,6 @@
       <c r="D30" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
@@ -1498,10 +1808,6 @@
       <c r="D31" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
@@ -1516,10 +1822,6 @@
       <c r="D32" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
@@ -1534,10 +1836,6 @@
       <c r="D33" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
@@ -1552,10 +1850,6 @@
       <c r="D34" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
@@ -1570,10 +1864,6 @@
       <c r="D35" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -1588,12 +1878,8 @@
       <c r="D36" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>57</v>
       </c>
@@ -1609,12 +1895,24 @@
       <c r="E37" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
+      <c r="F37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="L37" s="19"/>
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
@@ -1635,10 +1933,24 @@
       <c r="E38" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
+      <c r="F38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="K38" s="21" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
@@ -1656,10 +1968,24 @@
       <c r="E39" s="6">
         <v>1</v>
       </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
+      <c r="F39" s="6">
+        <v>1</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1</v>
+      </c>
+      <c r="H39" s="6">
+        <v>1</v>
+      </c>
+      <c r="I39" s="6">
+        <v>1</v>
+      </c>
+      <c r="J39" s="6">
+        <v>1</v>
+      </c>
+      <c r="K39" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -1677,10 +2003,24 @@
       <c r="E40" s="3">
         <v>9000</v>
       </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
+      <c r="F40" s="3">
+        <v>9000</v>
+      </c>
+      <c r="G40" s="3">
+        <v>9000</v>
+      </c>
+      <c r="H40" s="3">
+        <v>9000</v>
+      </c>
+      <c r="I40" s="3">
+        <v>9000</v>
+      </c>
+      <c r="J40" s="3">
+        <v>9000</v>
+      </c>
+      <c r="K40" s="3">
+        <v>9000</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
@@ -1696,12 +2036,26 @@
         <v>70</v>
       </c>
       <c r="E41" s="6">
-        <v>300000</v>
-      </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
+        <v>320000</v>
+      </c>
+      <c r="F41" s="6">
+        <v>320000</v>
+      </c>
+      <c r="G41" s="6">
+        <v>320000</v>
+      </c>
+      <c r="H41" s="3">
+        <v>30000</v>
+      </c>
+      <c r="I41" s="6">
+        <v>320000</v>
+      </c>
+      <c r="J41" s="6">
+        <v>320000</v>
+      </c>
+      <c r="K41" s="6">
+        <v>320000</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
@@ -1719,10 +2073,27 @@
       <c r="E42" s="6">
         <v>1</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+      <c r="F42" s="6">
+        <v>1</v>
+      </c>
+      <c r="G42" s="6">
+        <v>1</v>
+      </c>
+      <c r="H42" s="6">
+        <v>1</v>
+      </c>
+      <c r="I42" s="6">
+        <v>1</v>
+      </c>
+      <c r="J42" s="6">
+        <v>1</v>
+      </c>
+      <c r="K42" s="6">
+        <v>1</v>
+      </c>
+      <c r="M42" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
@@ -1740,10 +2111,27 @@
       <c r="E43" s="3">
         <v>1000</v>
       </c>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
+      <c r="F43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="K43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="M43" s="3">
+        <v>1000</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
@@ -1761,10 +2149,27 @@
       <c r="E44" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
+      <c r="F44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
@@ -1782,10 +2187,27 @@
       <c r="E45" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
+      <c r="F45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
@@ -1803,10 +2225,27 @@
       <c r="E46" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
+      <c r="F46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
@@ -1824,10 +2263,27 @@
       <c r="E47" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
+      <c r="F47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
@@ -1845,41 +2301,64 @@
       <c r="E48" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>12</v>
+      <c r="F48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="25"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="13" t="s">
-        <v>59</v>
-      </c>
+      <c r="D50" s="13"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A37:D50 A5:D22">
+  <conditionalFormatting sqref="A5:D22 A37:D50">
     <cfRule type="expression" dxfId="2" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
@@ -1895,7 +2374,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:N14" xr:uid="{2C70E2B3-8915-4AE7-992D-9B572ECD8046}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N14" xr:uid="{2C70E2B3-8915-4AE7-992D-9B572ECD8046}">
       <formula1>TEST_OUTCOME_TYPES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added additional documentation for the Ruletest JSON Generation guide markdown.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_tests_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_tests_draft.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44E1BE5-0A72-44FF-BF9F-A0FA7609A0E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD33A49D-7B61-4232-9062-9C474BDE539F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="9" r:id="rId1"/>
-    <sheet name="TCDs_dict" sheetId="8" r:id="rId2"/>
-    <sheet name="TCDs_arch" sheetId="6" r:id="rId3"/>
-    <sheet name="Lookups" sheetId="2" r:id="rId4"/>
+    <sheet name="TCDs_dict" sheetId="8" state="hidden" r:id="rId2"/>
+    <sheet name="TCDs_arch" sheetId="6" state="hidden" r:id="rId3"/>
+    <sheet name="Lookups" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="RMR_TYPES">Lookups!$B$2:$B$4</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="96">
   <si>
     <t>pass</t>
   </si>
@@ -1188,10 +1188,10 @@
   <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D67" sqref="D67"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,7 +1232,7 @@
         <v>rule-5-7a</v>
       </c>
       <c r="G1" s="3" t="str">
-        <f t="shared" ref="G1:N1" si="0">"rule-"&amp;G2&amp;"-"&amp;G3&amp;G4</f>
+        <f t="shared" ref="G1:I1" si="0">"rule-"&amp;G2&amp;"-"&amp;G3&amp;G4</f>
         <v>rule-5-7b</v>
       </c>
       <c r="H1" s="3" t="str">
@@ -1243,26 +1243,11 @@
         <f t="shared" si="0"/>
         <v>rule-5-7d</v>
       </c>
-      <c r="J1" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-5-7e</v>
-      </c>
-      <c r="K1" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-5-7f</v>
-      </c>
-      <c r="L1" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-5-7g</v>
-      </c>
-      <c r="M1" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-5-7h</v>
-      </c>
-      <c r="N1" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-5-7i</v>
-      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1283,21 +1268,6 @@
         <v>5</v>
       </c>
       <c r="I2" s="1">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1">
-        <v>5</v>
-      </c>
-      <c r="L2" s="1">
-        <v>5</v>
-      </c>
-      <c r="M2" s="1">
-        <v>5</v>
-      </c>
-      <c r="N2" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1321,21 +1291,6 @@
       <c r="I3" s="1">
         <v>7</v>
       </c>
-      <c r="J3" s="1">
-        <v>7</v>
-      </c>
-      <c r="K3" s="1">
-        <v>7</v>
-      </c>
-      <c r="L3" s="1">
-        <v>7</v>
-      </c>
-      <c r="M3" s="1">
-        <v>7</v>
-      </c>
-      <c r="N3" s="1">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -1357,21 +1312,7 @@
       <c r="I4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -1393,21 +1334,11 @@
       <c r="I5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1428,21 +1359,6 @@
         <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3203,8 +3119,9 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection activeCell="F41" sqref="F41:F56"/>
+      <selection pane="topRight" activeCell="F41" sqref="F41:F56"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41:F56"/>
       <selection pane="bottomRight" activeCell="F41" sqref="F41:F56"/>
     </sheetView>
   </sheetViews>
@@ -4433,9 +4350,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="G22" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H37" sqref="H37:H48"/>
+      <selection activeCell="F41" sqref="F41:F56"/>
+      <selection pane="topRight" activeCell="F41" sqref="F41:F56"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41:F56"/>
+      <selection pane="bottomRight" activeCell="F41" sqref="F41:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5922,7 +5840,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F41" sqref="F41:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>